<commit_message>
add api and api doc
</commit_message>
<xml_diff>
--- a/daydayup api.xlsx
+++ b/daydayup api.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="38340" windowHeight="21140" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="9760" yWindow="0" windowWidth="38340" windowHeight="21140" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="接口文档说明" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet name="Banner广告相关接口" sheetId="6" r:id="rId4"/>
     <sheet name="目标相关接口" sheetId="7" r:id="rId5"/>
     <sheet name="目标记录相关接口" sheetId="8" r:id="rId6"/>
+    <sheet name="督促目标相关接口" sheetId="9" r:id="rId7"/>
+    <sheet name="消息相关接口" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="237">
   <si>
     <t>1.获取验证码</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -735,6 +737,242 @@
   </si>
   <si>
     <t>4.取消点赞目标记录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>督促目标相关接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.督促目标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST /supervises/create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.接受督促</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST /supervises/:supervise_id/accept</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用示例：POST /supervises/12/accept</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.拒绝督促</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST /supervises/:supervise_id/refuse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用示例：POST /supervises/12/refuse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.更换目标督促人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST /supervises/destroy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消息相关接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.获取用户未读消息条数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET /messages/unread_count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用示例：GET /messages/unread_count?token=xxxxxx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.根据消息类别汇总消息列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET /messages/list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用示例：GET /messages/list?token=xxxxxx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.读某个消息类别下的消息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET /messages/read</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>message_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消息类别，值为：1,2,3,4中的一个，分别对应：系统消息，评论消息，加油消息，粉丝消息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>message_type=2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用示例：GET /messages/read?token=xxxxxx&amp;message_type=3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST /talks/send</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>聊天内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content=xxxxx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receiver_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消息接受者id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receiver_id=3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET /talks/read</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sender_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消息发送者id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sender_id=2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用示例：GET /talks/read?token=xxxxxx&amp;sender_id=3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.发送聊天信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.获取某个用户与我的聊天记录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.意见反馈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST /feedbacks/send</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>body</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>反馈内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>body=xxxxx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意：前端在展示聊天记录时，需要像QQ消息那样展示。可以通过比较sender_id与每一条聊天记录的sender_id进行比较，如果二者相等表示是我自己发布的消息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model=iPod4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>os</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>操作系统</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>os=iOS 8.1.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备语言</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lang=zh_CN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app当前版本号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>version=1.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备id，如果是iOS 可以使用open udid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uid=osAXCDD234kdddddd</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -883,8 +1121,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1107,7 +1383,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="173">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1175,6 +1451,25 @@
     <cellStyle name="超链接" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -1242,6 +1537,25 @@
     <cellStyle name="访问过的超链接" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1593,7 +1907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A71" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
@@ -3019,7 +3333,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A5" sqref="A5:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3154,6 +3468,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4502,8 +4817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:D45"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4997,4 +5312,1287 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+    <col min="4" max="4" width="65.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4" ht="48" customHeight="1">
+      <c r="A5" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:4" ht="45" customHeight="1">
+      <c r="A7" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:4" ht="44" customHeight="1">
+      <c r="A9" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+    </row>
+    <row r="11" spans="1:4" ht="33" customHeight="1">
+      <c r="A11" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="40" customHeight="1">
+      <c r="A12" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" customHeight="1">
+      <c r="A13" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" ht="48" customHeight="1">
+      <c r="A16" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="1:4" ht="45" customHeight="1">
+      <c r="A18" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+    </row>
+    <row r="20" spans="1:4" ht="44" customHeight="1">
+      <c r="A20" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+    </row>
+    <row r="22" spans="1:4" ht="33" customHeight="1">
+      <c r="A22" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" customHeight="1">
+      <c r="A23" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="40" customHeight="1">
+      <c r="A24" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="1:4" ht="43" customHeight="1">
+      <c r="A26" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="1:4" ht="48" customHeight="1">
+      <c r="A29" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+    </row>
+    <row r="31" spans="1:4" ht="45" customHeight="1">
+      <c r="A31" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+    </row>
+    <row r="33" spans="1:4" ht="44" customHeight="1">
+      <c r="A33" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="28"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+    </row>
+    <row r="35" spans="1:4" ht="33" customHeight="1">
+      <c r="A35" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" customHeight="1">
+      <c r="A36" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="40" customHeight="1">
+      <c r="A37" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:4" ht="43" customHeight="1">
+      <c r="A39" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+    </row>
+    <row r="42" spans="1:4" ht="48" customHeight="1">
+      <c r="A42" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+    </row>
+    <row r="44" spans="1:4" ht="45" customHeight="1">
+      <c r="A44" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+    </row>
+    <row r="46" spans="1:4" ht="44" customHeight="1">
+      <c r="A46" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="28"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+    </row>
+    <row r="48" spans="1:4" ht="33" customHeight="1">
+      <c r="A48" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="40" customHeight="1">
+      <c r="A49" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30" customHeight="1">
+      <c r="A50" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A40:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A1:D4"/>
+    <mergeCell ref="A14:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="58.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4" ht="48" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" ht="45" customHeight="1">
+      <c r="A7" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" ht="44" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" ht="33" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" customHeight="1">
+      <c r="A12" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:4" ht="44" customHeight="1">
+      <c r="A14" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:4" ht="48" customHeight="1">
+      <c r="A17" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" ht="45" customHeight="1">
+      <c r="A19" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" ht="44" customHeight="1">
+      <c r="A21" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" ht="33" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" customHeight="1">
+      <c r="A24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="1:4" ht="44" customHeight="1">
+      <c r="A26" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="1:4" ht="48" customHeight="1">
+      <c r="A29" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" ht="45" customHeight="1">
+      <c r="A31" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" ht="44" customHeight="1">
+      <c r="A33" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" ht="33" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" customHeight="1">
+      <c r="A36" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="83" customHeight="1">
+      <c r="A37" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:4" ht="44" customHeight="1">
+      <c r="A39" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+    </row>
+    <row r="42" spans="1:4" ht="48" customHeight="1">
+      <c r="A42" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+    </row>
+    <row r="44" spans="1:4" ht="45" customHeight="1">
+      <c r="A44" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+    </row>
+    <row r="46" spans="1:4" ht="44" customHeight="1">
+      <c r="A46" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="28"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+    </row>
+    <row r="48" spans="1:4" ht="33" customHeight="1">
+      <c r="A48" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="40" customHeight="1">
+      <c r="A49" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B49" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30" customHeight="1">
+      <c r="A50" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="30" customHeight="1">
+      <c r="A51" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+    </row>
+    <row r="54" spans="1:4" ht="48" customHeight="1">
+      <c r="A54" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+    </row>
+    <row r="56" spans="1:4" ht="45" customHeight="1">
+      <c r="A56" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="1:4" ht="44" customHeight="1">
+      <c r="A58" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+    </row>
+    <row r="60" spans="1:4" ht="33" customHeight="1">
+      <c r="A60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="30" customHeight="1">
+      <c r="A61" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="40" customHeight="1">
+      <c r="A62" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="11"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+    </row>
+    <row r="64" spans="1:4" ht="44" customHeight="1">
+      <c r="A64" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+    </row>
+    <row r="66" spans="1:4" ht="71" customHeight="1">
+      <c r="A66" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+    </row>
+    <row r="69" spans="1:4" ht="48" customHeight="1">
+      <c r="A69" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="20"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
+    </row>
+    <row r="71" spans="1:4" ht="45" customHeight="1">
+      <c r="A71" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="20"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
+    </row>
+    <row r="73" spans="1:4" ht="44" customHeight="1">
+      <c r="A73" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="28"/>
+      <c r="B74" s="28"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+    </row>
+    <row r="75" spans="1:4" ht="33" customHeight="1">
+      <c r="A75" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="40" customHeight="1">
+      <c r="A76" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B76" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="30" customHeight="1">
+      <c r="A77" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B77" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="30" customHeight="1">
+      <c r="A78" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B78" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="30" customHeight="1">
+      <c r="A79" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B79" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="30" customHeight="1">
+      <c r="A80" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B80" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="48" customHeight="1">
+      <c r="A81" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B81" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="11"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="12"/>
+      <c r="B83" s="12"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="53">
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A67:D68"/>
+    <mergeCell ref="A82:D83"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A52:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A40:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A27:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A1:D4"/>
+    <mergeCell ref="A15:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>